<commit_message>
Updated TensorRT notebook, README and images
</commit_message>
<xml_diff>
--- a/images/bert_performance.xlsx
+++ b/images/bert_performance.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/Documents/Github/bert-finetune/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F638F981-FC69-A24C-837F-95458BE9388F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7067B9B7-88EE-AA4B-9F96-A66B0390D846}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8B8067C8-0296-5D4C-86C0-A9E7EAFB1B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$44</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$45:$A$48</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$B$44</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$B$45:$B$48</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$C$44</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$C$45:$C$48</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -123,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,14 +143,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,15 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -3729,6 +3726,665 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="0" i="0">
+                <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t>Scaling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" b="0" i="0" baseline="0">
+                <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+              </a:rPr>
+              <a:t> Performance (BERTBASE)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1600" b="0" i="0">
+              <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V100 (16GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$45:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$B$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E0E-3748-8FFF-B046B7CDAD21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$44</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V100 (32GB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="76B900"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$45:$A$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$45:$C$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E0E-3748-8FFF-B046B7CDAD21}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-10"/>
+        <c:axId val="1558951376"/>
+        <c:axId val="1558980832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1558951376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1"/>
+                  <a:t>Number of V100</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1" baseline="0"/>
+                  <a:t> GPUs in NVLink</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37529116163850307"/>
+              <c:y val="0.89639909693036279"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1558980832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1558980832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="1"/>
+                  <a:t>Examples per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.5730337078651686E-2"/>
+              <c:y val="0.26441773768689691"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1558951376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0" i="0">
+          <a:latin typeface="DINPro" panose="02000503030000020004" pitchFamily="2" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3969,6 +4625,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6485,6 +7181,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7213,6 +8412,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>35983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>783167</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>148166</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C637271-95C0-D44B-86AF-B329AFE3CBBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7515,8 +8750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E751DE-BC54-3740-8EFA-CD1A254CABDE}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7870,7 +9105,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7886,8 +9121,11 @@
       <c r="A45" s="1">
         <v>1</v>
       </c>
+      <c r="B45">
+        <v>79</v>
+      </c>
       <c r="C45">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated README and images
</commit_message>
<xml_diff>
--- a/images/bert_performance.xlsx
+++ b/images/bert_performance.xlsx
@@ -8,21 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/Documents/Github/bert-finetune/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7067B9B7-88EE-AA4B-9F96-A66B0390D846}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF5B29-78F7-F54A-BF1A-90B64DC73895}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8B8067C8-0296-5D4C-86C0-A9E7EAFB1B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$44</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$45:$A$48</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$B$44</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$B$45:$B$48</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$C$44</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$C$45:$C$48</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>BERT Performance Comparisons</t>
   </si>
@@ -124,7 +116,13 @@
     <t>Avg NVLink BW</t>
   </si>
   <si>
-    <t>Examples/s</t>
+    <t>8×V100 (16GB)</t>
+  </si>
+  <si>
+    <t>8×V100 (32GB)</t>
+  </si>
+  <si>
+    <t>Examples/s on 8×V100 (16GB)</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1107,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V100 (16GB)</c:v>
+                  <c:v>8×V100 (16GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1238,7 +1236,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V100 (32GB)</c:v>
+                  <c:v>8×V100 (32GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1745,7 +1743,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V100 (16GB)</c:v>
+                  <c:v>8×V100 (16GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1854,7 +1852,7 @@
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>104</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1874,7 +1872,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>V100 (32GB)</c:v>
+                  <c:v>8×V100 (32GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2381,7 +2379,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Examples/s</c:v>
+                  <c:v>Examples/s on 8×V100 (16GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3097,7 +3095,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Examples/s</c:v>
+                  <c:v>Examples/s on 8×V100 (16GB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8750,8 +8748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E751DE-BC54-3740-8EFA-CD1A254CABDE}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8855,7 +8853,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>153</v>
@@ -8872,7 +8870,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>168</v>
@@ -8920,7 +8918,7 @@
         <v>74</v>
       </c>
       <c r="E22">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -8961,7 +8959,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>298</v>
@@ -9031,7 +9029,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>71</v>

</xml_diff>